<commit_message>
Add budget search and fix salvage value computations
</commit_message>
<xml_diff>
--- a/Inputs/inputs.xlsx
+++ b/Inputs/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/microgrid_MP/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{353AE6E4-AFA5-4B68-AD1B-B2C80ADE73C4}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB443246-B432-468B-B429-D670C10072ED}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>241300</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -643,16 +643,16 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -724,7 +724,7 @@
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>241300</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>6350</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -749,7 +749,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -794,15 +794,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -903,12 +903,12 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" customWidth="1"/>
     <col min="2" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1153,8 +1153,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1245,13 +1245,13 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="5.6328125" customWidth="1"/>
+    <col min="2" max="25" width="5.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -1575,7 +1575,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
+    <col min="2" max="25" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -1975,13 +1975,13 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="25" width="6.6328125" customWidth="1"/>
+    <col min="2" max="25" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update code with new salvage and constrained demand
</commit_message>
<xml_diff>
--- a/Inputs/inputs.xlsx
+++ b/Inputs/inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/microgrid_MP/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB443246-B432-468B-B429-D670C10072ED}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{390FEF1A-0375-45EE-A2D6-6C903961C6D6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -320,6 +320,10 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2398,6 +2402,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D835CF4C7D56B243BA013D4D2E10914B" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e645ef68b9493f2ee8bae9e534bc24f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6d4e152b-60f6-4719-8921-68b5b8011cde" xmlns:ns4="28683373-984a-4841-9f0e-018f3f7bab1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a06da6e71fc3d3bdf7cbe176c2a8afa1" ns3:_="" ns4:_="">
     <xsd:import namespace="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
@@ -2650,15 +2663,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
   <ds:schemaRefs>
@@ -2677,6 +2681,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE4FBA5-6C26-4B97-9218-92B658F853C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2693,12 +2705,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add UD penalty in code
</commit_message>
<xml_diff>
--- a/Inputs/inputs.xlsx
+++ b/Inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/microgrid_MP/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{390FEF1A-0375-45EE-A2D6-6C903961C6D6}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{AAD2F7EF-0845-4A2E-9423-0E1C0E08F108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D88A2A3-228E-4405-8330-01EE10F5E7F5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>241300</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -650,17 +650,17 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.02</v>
       </c>
@@ -726,9 +726,9 @@
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>241300</xdr:colOff>
+                    <xdr:colOff>238125</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -750,14 +750,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -765,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -801,17 +801,17 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -828,7 +828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -848,7 +848,7 @@
         <v>1.4000710227272728E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -888,7 +888,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -904,20 +904,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" customWidth="1"/>
-    <col min="2" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -928,7 +928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -942,7 +942,7 @@
         <v>335.12299999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -956,7 +956,7 @@
         <v>323.07068600000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -970,7 +970,7 @@
         <v>310.63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -984,7 +984,7 @@
         <v>298.57800000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -998,7 +998,7 @@
         <v>286.52600000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>274.08500000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>269.80900000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>265.92099999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>261.64400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>257.36799999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>253.09100000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>249.20400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>244.92699999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>240.65100000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1136,6 +1136,20 @@
       </c>
       <c r="D16">
         <v>236.374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>800</v>
+      </c>
+      <c r="C17">
+        <v>652.61800000000005</v>
+      </c>
+      <c r="D17">
+        <v>232.48699999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1154,19 +1168,19 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1175,7 +1189,7 @@
         <v>0.34800785000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1198,7 @@
         <v>0.26788265000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1207,14 +1221,14 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1222,7 +1236,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1230,7 +1244,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1252,13 +1266,13 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="5.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -1332,7 +1346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1409,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -1486,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1577,12 +1591,12 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="25" width="6.54296875" customWidth="1"/>
+    <col min="2" max="25" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -1656,7 +1670,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1733,7 +1747,7 @@
         <v>0.57693786350230403</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1824,7 @@
         <v>0.39380200730040377</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1887,84 +1901,84 @@
         <v>0.32997560070809001</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
@@ -1979,16 +1993,16 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="25" width="6.54296875" customWidth="1"/>
+    <col min="2" max="25" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -2062,7 +2076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2139,7 +2153,7 @@
         <v>0.62185117302052784</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2216,7 +2230,7 @@
         <v>0.19264757142857142</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2293,97 +2307,97 @@
         <v>0.3463776522754351</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
@@ -2394,23 +2408,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D835CF4C7D56B243BA013D4D2E10914B" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e645ef68b9493f2ee8bae9e534bc24f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6d4e152b-60f6-4719-8921-68b5b8011cde" xmlns:ns4="28683373-984a-4841-9f0e-018f3f7bab1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a06da6e71fc3d3bdf7cbe176c2a8afa1" ns3:_="" ns4:_="">
     <xsd:import namespace="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
@@ -2663,32 +2660,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE4FBA5-6C26-4B97-9218-92B658F853C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2705,4 +2694,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>